<commit_message>
Updated Cotton Starting Point
</commit_message>
<xml_diff>
--- a/Prototypes/Cotton/Observed.xlsx
+++ b/Prototypes/Cotton/Observed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr showPivotChartFilter="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX\Prototypes\Cotton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Prototypes\Cotton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87695A0-7BBC-471A-8725-A85522A371B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7607055B-401C-449F-8AFF-37E578AF56D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="16608" windowHeight="10536" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="14" r:id="rId1"/>
@@ -171,24 +171,6 @@
     <t>PodsPerPlant</t>
   </si>
   <si>
-    <t>GriffithSowNov15CvHooper_MG40</t>
-  </si>
-  <si>
-    <t>GriffithSowDec08CvHooper_MG40</t>
-  </si>
-  <si>
-    <t>GriffithSowJan06CvHooper_MG40</t>
-  </si>
-  <si>
-    <t>GriffithSowNov15CvStephens_MG40</t>
-  </si>
-  <si>
-    <t>GriffithSowDec08CvStephens_MG40</t>
-  </si>
-  <si>
-    <t>GriffithSowJan06CvStephens_MG40</t>
-  </si>
-  <si>
     <t>nodes_per_main_stem</t>
   </si>
   <si>
@@ -343,6 +325,24 @@
   </si>
   <si>
     <t>Cotton.Root.Depth</t>
+  </si>
+  <si>
+    <t>Burdekin2008SowNov15CvStephens_MG40</t>
+  </si>
+  <si>
+    <t>Burdekin2008SowNov15CvHooper_MG40</t>
+  </si>
+  <si>
+    <t>Burdekin2008SowDec08CvStephens_MG40</t>
+  </si>
+  <si>
+    <t>Burdekin2008SowDec08CvHooper_MG40</t>
+  </si>
+  <si>
+    <t>Burdekin2008SowJan06CvStephens_MG40</t>
+  </si>
+  <si>
+    <t>Burdekin2008SowJan06CvHooper_MG40</t>
   </si>
 </sst>
 </file>
@@ -422,26 +422,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -798,98 +797,98 @@
   <dimension ref="A1:CR377"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10716" ySplit="576" topLeftCell="Q1"/>
+      <pane xSplit="10710" ySplit="570" topLeftCell="Q2" activePane="bottomLeft"/>
       <selection sqref="A1:XFD1"/>
       <selection pane="topRight" activeCell="R1" sqref="R1:R1048576"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A59"/>
       <selection pane="bottomRight" activeCell="Q225" sqref="Q225"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="1" max="1" width="43.3125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.3125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3125" customWidth="1"/>
+    <col min="1" max="1" width="43.29296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.29296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.29296875" customWidth="1"/>
     <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
-    <col min="6" max="6" width="28.89453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.68359375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.87890625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.89453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1015625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.3125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.1015625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.68359375" customWidth="1"/>
-    <col min="14" max="14" width="14.1015625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.3125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.87890625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1171875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.29296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1171875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.703125" customWidth="1"/>
+    <col min="14" max="14" width="14.1171875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.29296875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.41796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.68359375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.68359375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.1015625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.89453125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.89453125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.41796875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.41796875" customWidth="1"/>
-    <col min="25" max="25" width="15.1015625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.41015625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.1171875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.87890625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.87890625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.41015625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.41015625" customWidth="1"/>
+    <col min="25" max="25" width="15.1171875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" customWidth="1"/>
-    <col min="28" max="29" width="21.89453125" customWidth="1"/>
-    <col min="30" max="30" width="20.5234375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.68359375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21.68359375" customWidth="1"/>
-    <col min="33" max="33" width="17.68359375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.41796875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.3125" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="21.87890625" customWidth="1"/>
+    <col min="30" max="30" width="20.52734375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.703125" customWidth="1"/>
+    <col min="33" max="33" width="17.703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.41015625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.29296875" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="18" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.5234375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.68359375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="17.68359375" customWidth="1"/>
-    <col min="40" max="40" width="13.68359375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.68359375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.3125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.52734375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.703125" customWidth="1"/>
+    <col min="40" max="40" width="13.703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.703125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13.29296875" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="14" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="20.68359375" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="46" width="20.68359375" customWidth="1"/>
-    <col min="47" max="47" width="9.3125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.68359375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="13.89453125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="20.703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="46" width="20.703125" customWidth="1"/>
+    <col min="47" max="47" width="9.29296875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="13.87890625" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="17" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="5.68359375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="8.1015625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="5.703125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="8.1171875" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="14" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="14.3125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="10.68359375" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="10.5234375" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="6.5234375" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="7.5234375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="14.89453125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="17.41796875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="14.1015625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="15.1015625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="14.68359375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="14.29296875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="10.703125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="10.52734375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="6.52734375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="7.52734375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="14.87890625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="17.41015625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14.1171875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="15.1171875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="14.703125" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="15" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="11.68359375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="11.3125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="17.68359375" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="20.3125" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="18.41796875" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="17.3125" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="17.41796875" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="18.1015625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="13.68359375" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="16.3125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="14.1015625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="14.41796875" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="13.89453125" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="10.68359375" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="18.68359375" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="13.41796875" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="18.68359375" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="11.703125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="11.29296875" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="17.703125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="20.29296875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="18.41015625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="17.29296875" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="17.41015625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="18.1171875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="13.703125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="16.29296875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="14.1171875" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="14.41015625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="13.87890625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="10.703125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="18.703125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="13.41015625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="18.703125" bestFit="1" customWidth="1"/>
     <col min="82" max="82" width="18" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="10.89453125" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="9.89453125" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="12.1015625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="10.87890625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="9.87890625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="12.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:96">
@@ -900,22 +899,22 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
@@ -924,112 +923,112 @@
         <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="L1" t="s">
         <v>44</v>
       </c>
       <c r="M1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="N1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="O1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="P1" t="s">
         <v>43</v>
       </c>
       <c r="Q1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" t="s">
+        <v>70</v>
+      </c>
+      <c r="T1" t="s">
+        <v>71</v>
+      </c>
+      <c r="U1" t="s">
+        <v>72</v>
+      </c>
+      <c r="V1" t="s">
+        <v>73</v>
+      </c>
+      <c r="W1" t="s">
         <v>74</v>
       </c>
-      <c r="R1" t="s">
+      <c r="X1" t="s">
         <v>75</v>
       </c>
-      <c r="S1" t="s">
+      <c r="Y1" t="s">
         <v>76</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Z1" t="s">
         <v>77</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AA1" t="s">
         <v>78</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AB1" t="s">
         <v>79</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AC1" t="s">
         <v>80</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AD1" t="s">
         <v>81</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AE1" t="s">
         <v>82</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AF1" t="s">
         <v>83</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AG1" t="s">
         <v>84</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AH1" t="s">
         <v>85</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AI1" t="s">
         <v>86</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AJ1" t="s">
         <v>87</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AK1" t="s">
         <v>88</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AL1" t="s">
         <v>89</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AM1" t="s">
         <v>90</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AN1" t="s">
         <v>91</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AO1" t="s">
         <v>92</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AP1" t="s">
         <v>93</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AQ1" t="s">
         <v>94</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AR1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="AM1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AR1" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="AS1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="AT1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="AU1" t="s">
         <v>4</v>
@@ -1041,7 +1040,7 @@
         <v>6</v>
       </c>
       <c r="AX1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="AY1" t="s">
         <v>7</v>
@@ -1149,42 +1148,42 @@
         <v>41</v>
       </c>
       <c r="CH1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="CI1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="CJ1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="CK1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="CL1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>50</v>
+      </c>
+      <c r="CN1" t="s">
         <v>51</v>
       </c>
-      <c r="CI1" s="5" t="s">
+      <c r="CO1" t="s">
         <v>52</v>
       </c>
-      <c r="CJ1" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="CK1" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="CL1" s="5" t="s">
+      <c r="CP1" t="s">
         <v>55</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CQ1" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CR1" s="20" t="s">
         <v>57</v>
-      </c>
-      <c r="CO1" t="s">
-        <v>58</v>
-      </c>
-      <c r="CP1" t="s">
-        <v>61</v>
-      </c>
-      <c r="CQ1" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="CR1" s="21" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:96">
       <c r="A2" s="4" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="B2" s="2">
         <v>36508</v>
@@ -1199,7 +1198,7 @@
     </row>
     <row r="3" spans="1:96">
       <c r="A3" s="4" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="B3" s="2">
         <v>36522</v>
@@ -1214,7 +1213,7 @@
     </row>
     <row r="4" spans="1:96">
       <c r="A4" s="4" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="B4" s="2">
         <v>36530</v>
@@ -1229,7 +1228,7 @@
     </row>
     <row r="5" spans="1:96">
       <c r="A5" s="4" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="B5" s="2">
         <v>36536</v>
@@ -1244,7 +1243,7 @@
     </row>
     <row r="6" spans="1:96">
       <c r="A6" s="4" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="B6" s="2">
         <v>36543</v>
@@ -1259,7 +1258,7 @@
     </row>
     <row r="7" spans="1:96">
       <c r="A7" s="4" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="B7" s="2">
         <v>36549</v>
@@ -1277,7 +1276,7 @@
     </row>
     <row r="8" spans="1:96">
       <c r="A8" s="4" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="B8" s="2">
         <v>36563</v>
@@ -1295,7 +1294,7 @@
     </row>
     <row r="9" spans="1:96">
       <c r="A9" s="4" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="B9" s="2">
         <v>36577</v>
@@ -1313,7 +1312,7 @@
     </row>
     <row r="10" spans="1:96">
       <c r="A10" s="4" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="B10" s="2">
         <v>36593</v>
@@ -1331,7 +1330,7 @@
     </row>
     <row r="11" spans="1:96">
       <c r="A11" s="4" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="B11" s="2">
         <v>36607</v>
@@ -1349,7 +1348,7 @@
     </row>
     <row r="12" spans="1:96">
       <c r="A12" s="4" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="B12" s="2">
         <v>36621</v>
@@ -1382,7 +1381,7 @@
     </row>
     <row r="13" spans="1:96">
       <c r="A13" s="4" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="B13" s="2">
         <v>36523</v>
@@ -1394,7 +1393,7 @@
     </row>
     <row r="14" spans="1:96">
       <c r="A14" s="4" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="B14" s="2">
         <v>36532</v>
@@ -1409,7 +1408,7 @@
     </row>
     <row r="15" spans="1:96">
       <c r="A15" s="4" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="B15" s="2">
         <v>36537</v>
@@ -1424,7 +1423,7 @@
     </row>
     <row r="16" spans="1:96">
       <c r="A16" s="4" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="B16" s="2">
         <v>36550</v>
@@ -1442,7 +1441,7 @@
     </row>
     <row r="17" spans="1:29">
       <c r="A17" s="4" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="B17" s="2">
         <v>36565</v>
@@ -1460,7 +1459,7 @@
     </row>
     <row r="18" spans="1:29">
       <c r="A18" s="4" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="B18" s="2">
         <v>36578</v>
@@ -1475,7 +1474,7 @@
     </row>
     <row r="19" spans="1:29">
       <c r="A19" s="4" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="B19" s="2">
         <v>36593</v>
@@ -1490,7 +1489,7 @@
     </row>
     <row r="20" spans="1:29">
       <c r="A20" s="4" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="B20" s="2">
         <v>36607</v>
@@ -1508,7 +1507,7 @@
     </row>
     <row r="21" spans="1:29">
       <c r="A21" s="4" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="B21" s="2">
         <v>36621</v>
@@ -1541,7 +1540,7 @@
     </row>
     <row r="22" spans="1:29">
       <c r="A22" s="4" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="B22" s="2">
         <v>36530</v>
@@ -1556,7 +1555,7 @@
     </row>
     <row r="23" spans="1:29">
       <c r="A23" s="4" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="B23" s="2">
         <v>36543</v>
@@ -1571,7 +1570,7 @@
     </row>
     <row r="24" spans="1:29">
       <c r="A24" s="4" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="B24" s="2">
         <v>36545</v>
@@ -1586,7 +1585,7 @@
     </row>
     <row r="25" spans="1:29">
       <c r="A25" s="4" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="B25" s="2">
         <v>36557</v>
@@ -1604,7 +1603,7 @@
     </row>
     <row r="26" spans="1:29">
       <c r="A26" s="4" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="B26" s="2">
         <v>36565</v>
@@ -1622,7 +1621,7 @@
     </row>
     <row r="27" spans="1:29">
       <c r="A27" s="4" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="B27" s="2">
         <v>36572</v>
@@ -1640,7 +1639,7 @@
     </row>
     <row r="28" spans="1:29">
       <c r="A28" s="4" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="B28" s="2">
         <v>36588</v>
@@ -1658,7 +1657,7 @@
     </row>
     <row r="29" spans="1:29">
       <c r="A29" s="4" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="B29" s="2">
         <v>36600</v>
@@ -1676,7 +1675,7 @@
     </row>
     <row r="30" spans="1:29">
       <c r="A30" s="4" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="B30" s="2">
         <v>36613</v>
@@ -1698,7 +1697,7 @@
     </row>
     <row r="31" spans="1:29">
       <c r="A31" s="4" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="B31" s="2">
         <v>36626</v>
@@ -1724,7 +1723,7 @@
     </row>
     <row r="32" spans="1:29">
       <c r="A32" s="4" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="B32" s="2">
         <v>36530</v>
@@ -1736,7 +1735,7 @@
     </row>
     <row r="33" spans="1:29">
       <c r="A33" s="4" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="B33" s="2">
         <v>36544</v>
@@ -1751,7 +1750,7 @@
     </row>
     <row r="34" spans="1:29">
       <c r="A34" s="4" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="B34" s="2">
         <v>36599</v>
@@ -1763,7 +1762,7 @@
     </row>
     <row r="35" spans="1:29">
       <c r="A35" s="4" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="B35" s="2">
         <v>36558</v>
@@ -1778,7 +1777,7 @@
     </row>
     <row r="36" spans="1:29">
       <c r="A36" s="4" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="B36" s="2">
         <v>36572</v>
@@ -1796,7 +1795,7 @@
     </row>
     <row r="37" spans="1:29">
       <c r="A37" s="4" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="B37" s="2">
         <v>36576</v>
@@ -1814,7 +1813,7 @@
     </row>
     <row r="38" spans="1:29">
       <c r="A38" s="4" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="B38" s="2">
         <v>36589</v>
@@ -1832,7 +1831,7 @@
     </row>
     <row r="39" spans="1:29">
       <c r="A39" s="4" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="B39" s="2">
         <v>36600</v>
@@ -1850,7 +1849,7 @@
     </row>
     <row r="40" spans="1:29">
       <c r="A40" s="4" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="B40" s="2">
         <v>36612</v>
@@ -1868,7 +1867,7 @@
     </row>
     <row r="41" spans="1:29">
       <c r="A41" s="4" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="B41" s="2">
         <v>36627</v>
@@ -1901,7 +1900,7 @@
     </row>
     <row r="42" spans="1:29">
       <c r="A42" s="4" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="B42" s="2">
         <v>36553</v>
@@ -1916,7 +1915,7 @@
     </row>
     <row r="43" spans="1:29">
       <c r="A43" s="4" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="B43" s="2">
         <v>36558</v>
@@ -1931,7 +1930,7 @@
     </row>
     <row r="44" spans="1:29">
       <c r="A44" s="4" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="B44" s="2">
         <v>36567</v>
@@ -1946,7 +1945,7 @@
     </row>
     <row r="45" spans="1:29">
       <c r="A45" s="4" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="B45" s="2">
         <v>36572</v>
@@ -1961,7 +1960,7 @@
     </row>
     <row r="46" spans="1:29">
       <c r="A46" s="4" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="B46" s="2">
         <v>36579</v>
@@ -1979,7 +1978,7 @@
     </row>
     <row r="47" spans="1:29">
       <c r="A47" s="4" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="B47" s="2">
         <v>36589</v>
@@ -1997,7 +1996,7 @@
     </row>
     <row r="48" spans="1:29">
       <c r="A48" s="4" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="B48" s="2">
         <v>36600</v>
@@ -2015,7 +2014,7 @@
     </row>
     <row r="49" spans="1:29">
       <c r="A49" s="4" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="B49" s="2">
         <v>36613</v>
@@ -2033,7 +2032,7 @@
     </row>
     <row r="50" spans="1:29">
       <c r="A50" s="4" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="B50" s="2">
         <v>36626</v>
@@ -2051,7 +2050,7 @@
     </row>
     <row r="51" spans="1:29">
       <c r="A51" s="4" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="B51" s="2">
         <v>36642</v>
@@ -2084,7 +2083,7 @@
     </row>
     <row r="52" spans="1:29">
       <c r="A52" s="4" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="B52" s="2">
         <v>36558</v>
@@ -2096,7 +2095,7 @@
     </row>
     <row r="53" spans="1:29">
       <c r="A53" s="4" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="B53" s="2">
         <v>36566</v>
@@ -2111,7 +2110,7 @@
     </row>
     <row r="54" spans="1:29">
       <c r="A54" s="4" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="B54" s="2">
         <v>36571</v>
@@ -2123,7 +2122,7 @@
     </row>
     <row r="55" spans="1:29">
       <c r="A55" s="4" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="B55" s="2">
         <v>36587</v>
@@ -2141,7 +2140,7 @@
     </row>
     <row r="56" spans="1:29">
       <c r="A56" s="4" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="B56" s="2">
         <v>36598</v>
@@ -2159,7 +2158,7 @@
     </row>
     <row r="57" spans="1:29">
       <c r="A57" s="4" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="B57" s="2">
         <v>36612</v>
@@ -2177,7 +2176,7 @@
     </row>
     <row r="58" spans="1:29">
       <c r="A58" s="4" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="B58" s="2">
         <v>36626</v>
@@ -2195,7 +2194,7 @@
     </row>
     <row r="59" spans="1:29">
       <c r="A59" s="4" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="B59" s="2">
         <v>36641</v>
@@ -2227,7 +2226,7 @@
       </c>
     </row>
     <row r="60" spans="1:29" s="5" customFormat="1">
-      <c r="A60" s="9"/>
+      <c r="A60" s="8"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
       <c r="K60"/>
@@ -2238,7 +2237,7 @@
       <c r="X60"/>
     </row>
     <row r="61" spans="1:29" s="5" customFormat="1">
-      <c r="A61" s="9"/>
+      <c r="A61" s="8"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
       <c r="K61"/>
@@ -2249,7 +2248,7 @@
       <c r="X61"/>
     </row>
     <row r="62" spans="1:29" s="5" customFormat="1">
-      <c r="A62" s="9"/>
+      <c r="A62" s="8"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
       <c r="K62"/>
@@ -2260,7 +2259,7 @@
       <c r="X62"/>
     </row>
     <row r="63" spans="1:29" s="5" customFormat="1">
-      <c r="A63" s="9"/>
+      <c r="A63" s="8"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
       <c r="K63"/>
@@ -2271,7 +2270,7 @@
       <c r="X63"/>
     </row>
     <row r="64" spans="1:29" s="5" customFormat="1">
-      <c r="A64" s="9"/>
+      <c r="A64" s="8"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
       <c r="K64"/>
@@ -2282,7 +2281,7 @@
       <c r="X64"/>
     </row>
     <row r="65" spans="1:46" s="5" customFormat="1">
-      <c r="A65" s="9"/>
+      <c r="A65" s="8"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
       <c r="K65"/>
@@ -2293,7 +2292,7 @@
       <c r="X65"/>
     </row>
     <row r="66" spans="1:46" s="5" customFormat="1">
-      <c r="A66" s="9"/>
+      <c r="A66" s="8"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
       <c r="K66"/>
@@ -2303,7 +2302,7 @@
       <c r="X66"/>
     </row>
     <row r="67" spans="1:46" s="5" customFormat="1">
-      <c r="A67" s="9"/>
+      <c r="A67" s="8"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
       <c r="K67"/>
@@ -2317,7 +2316,7 @@
       <c r="AC67"/>
     </row>
     <row r="68" spans="1:46" s="5" customFormat="1">
-      <c r="A68" s="9"/>
+      <c r="A68" s="8"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
       <c r="K68"/>
@@ -2330,7 +2329,7 @@
       <c r="AA68"/>
     </row>
     <row r="69" spans="1:46" s="5" customFormat="1">
-      <c r="A69" s="9"/>
+      <c r="A69" s="8"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
       <c r="K69"/>
@@ -2343,7 +2342,7 @@
       <c r="AA69"/>
     </row>
     <row r="70" spans="1:46" s="5" customFormat="1">
-      <c r="A70" s="9"/>
+      <c r="A70" s="8"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
       <c r="K70"/>
@@ -2356,12 +2355,12 @@
       <c r="AA70"/>
     </row>
     <row r="71" spans="1:46" s="5" customFormat="1">
-      <c r="A71" s="9"/>
+      <c r="A71" s="8"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
       <c r="E71" s="6"/>
-      <c r="H71" s="10"/>
+      <c r="H71" s="9"/>
       <c r="AC71"/>
     </row>
     <row r="72" spans="1:46">
@@ -2417,8 +2416,8 @@
       <c r="X79"/>
       <c r="Z79"/>
       <c r="AA79"/>
-      <c r="AB79" s="7"/>
-      <c r="AC79" s="7"/>
+      <c r="AB79"/>
+      <c r="AC79"/>
       <c r="AD79"/>
       <c r="AE79"/>
       <c r="AF79"/>
@@ -2431,255 +2430,177 @@
     <row r="80" spans="1:46">
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
-      <c r="AB80" s="7"/>
-      <c r="AC80" s="7"/>
-    </row>
-    <row r="81" spans="2:29">
+    </row>
+    <row r="81" spans="2:17">
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
-      <c r="AB81" s="7"/>
-      <c r="AC81" s="7"/>
-    </row>
-    <row r="82" spans="2:29">
+    </row>
+    <row r="82" spans="2:17">
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
-      <c r="AB82" s="7"/>
-      <c r="AC82" s="7"/>
-    </row>
-    <row r="83" spans="2:29">
+    </row>
+    <row r="83" spans="2:17">
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
-      <c r="AB83" s="7"/>
-      <c r="AC83" s="7"/>
-    </row>
-    <row r="84" spans="2:29">
+    </row>
+    <row r="84" spans="2:17">
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
-      <c r="AB84" s="7"/>
-      <c r="AC84" s="7"/>
-    </row>
-    <row r="85" spans="2:29">
+    </row>
+    <row r="85" spans="2:17">
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
-      <c r="AB85" s="7"/>
-      <c r="AC85" s="7"/>
-    </row>
-    <row r="86" spans="2:29">
+    </row>
+    <row r="86" spans="2:17">
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
-      <c r="AB86" s="7"/>
-      <c r="AC86" s="7"/>
-    </row>
-    <row r="87" spans="2:29">
+    </row>
+    <row r="87" spans="2:17">
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
-      <c r="AB87" s="7"/>
-      <c r="AC87" s="7"/>
-    </row>
-    <row r="88" spans="2:29" s="5" customFormat="1">
+    </row>
+    <row r="88" spans="2:17" s="5" customFormat="1">
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
     </row>
-    <row r="89" spans="2:29">
+    <row r="89" spans="2:17">
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="Q89" s="5"/>
-      <c r="AB89" s="7"/>
-      <c r="AC89" s="7"/>
-    </row>
-    <row r="90" spans="2:29">
+    </row>
+    <row r="90" spans="2:17">
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
-      <c r="AB90" s="7"/>
-      <c r="AC90" s="7"/>
-    </row>
-    <row r="91" spans="2:29">
+    </row>
+    <row r="91" spans="2:17">
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
-      <c r="AB91" s="7"/>
-      <c r="AC91" s="7"/>
-    </row>
-    <row r="92" spans="2:29">
+    </row>
+    <row r="92" spans="2:17">
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
-      <c r="AB92" s="7"/>
-      <c r="AC92" s="7"/>
-    </row>
-    <row r="93" spans="2:29">
+    </row>
+    <row r="93" spans="2:17">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
-      <c r="AB93" s="7"/>
-      <c r="AC93" s="7"/>
-    </row>
-    <row r="94" spans="2:29">
+    </row>
+    <row r="94" spans="2:17">
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
-      <c r="AB94" s="7"/>
-      <c r="AC94" s="7"/>
-    </row>
-    <row r="95" spans="2:29">
+    </row>
+    <row r="95" spans="2:17">
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
-      <c r="AB95" s="7"/>
-      <c r="AC95" s="7"/>
-    </row>
-    <row r="96" spans="2:29">
+    </row>
+    <row r="96" spans="2:17">
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
-      <c r="AB96" s="7"/>
-      <c r="AC96" s="7"/>
-    </row>
-    <row r="97" spans="2:29">
+    </row>
+    <row r="97" spans="2:17">
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
-      <c r="AB97" s="7"/>
-      <c r="AC97" s="7"/>
-    </row>
-    <row r="98" spans="2:29">
+    </row>
+    <row r="98" spans="2:17">
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
-      <c r="AB98" s="7"/>
-      <c r="AC98" s="7"/>
-    </row>
-    <row r="99" spans="2:29" s="5" customFormat="1">
+    </row>
+    <row r="99" spans="2:17" s="5" customFormat="1">
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
     </row>
-    <row r="100" spans="2:29">
+    <row r="100" spans="2:17">
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="Q100" s="5"/>
-      <c r="AB100" s="7"/>
-      <c r="AC100" s="7"/>
-    </row>
-    <row r="101" spans="2:29">
+    </row>
+    <row r="101" spans="2:17">
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
-      <c r="AB101" s="7"/>
-      <c r="AC101" s="7"/>
-    </row>
-    <row r="102" spans="2:29">
+    </row>
+    <row r="102" spans="2:17">
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
-      <c r="AB102" s="7"/>
-      <c r="AC102" s="7"/>
-    </row>
-    <row r="103" spans="2:29">
+    </row>
+    <row r="103" spans="2:17">
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
-      <c r="AB103" s="7"/>
-      <c r="AC103" s="7"/>
-    </row>
-    <row r="104" spans="2:29">
+    </row>
+    <row r="104" spans="2:17">
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="Q104" s="5"/>
-      <c r="AB104" s="7"/>
-      <c r="AC104" s="7"/>
-    </row>
-    <row r="105" spans="2:29">
+    </row>
+    <row r="105" spans="2:17">
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
-      <c r="AB105" s="7"/>
-      <c r="AC105" s="7"/>
-    </row>
-    <row r="106" spans="2:29">
+    </row>
+    <row r="106" spans="2:17">
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
-      <c r="AB106" s="7"/>
-      <c r="AC106" s="7"/>
-    </row>
-    <row r="107" spans="2:29">
+    </row>
+    <row r="107" spans="2:17">
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
-      <c r="AB107" s="7"/>
-      <c r="AC107" s="7"/>
-    </row>
-    <row r="108" spans="2:29">
+    </row>
+    <row r="108" spans="2:17">
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
-      <c r="AB108" s="7"/>
-      <c r="AC108" s="7"/>
-    </row>
-    <row r="109" spans="2:29">
+    </row>
+    <row r="109" spans="2:17">
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
-      <c r="AB109" s="7"/>
-      <c r="AC109" s="7"/>
-    </row>
-    <row r="110" spans="2:29">
+    </row>
+    <row r="110" spans="2:17">
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
       <c r="Q110" s="5"/>
-      <c r="AB110" s="7"/>
-    </row>
-    <row r="111" spans="2:29">
+    </row>
+    <row r="111" spans="2:17">
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
       <c r="Q111" s="5"/>
-      <c r="AB111" s="7"/>
-      <c r="AC111" s="7"/>
-    </row>
-    <row r="112" spans="2:29">
+    </row>
+    <row r="112" spans="2:17">
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
-      <c r="AB112" s="7"/>
-      <c r="AC112" s="7"/>
     </row>
     <row r="113" spans="1:46">
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
-      <c r="AB113" s="7"/>
-      <c r="AC113" s="7"/>
     </row>
     <row r="114" spans="1:46">
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="Q114" s="5"/>
-      <c r="AB114" s="7"/>
-      <c r="AC114" s="7"/>
     </row>
     <row r="115" spans="1:46">
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
-      <c r="AB115" s="7"/>
-      <c r="AC115" s="7"/>
     </row>
     <row r="116" spans="1:46">
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
-      <c r="AB116" s="7"/>
-      <c r="AC116" s="7"/>
     </row>
     <row r="117" spans="1:46">
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
-      <c r="AB117" s="7"/>
-      <c r="AC117" s="7"/>
     </row>
     <row r="118" spans="1:46">
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
-      <c r="AB118" s="7"/>
-      <c r="AC118" s="7"/>
     </row>
     <row r="119" spans="1:46">
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
-      <c r="AB119" s="7"/>
-      <c r="AC119" s="7"/>
     </row>
     <row r="120" spans="1:46">
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
-      <c r="AB120" s="7"/>
-      <c r="AC120" s="7"/>
     </row>
     <row r="121" spans="1:46">
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
       <c r="Q121" s="5"/>
-      <c r="AB121" s="7"/>
     </row>
     <row r="122" spans="1:46">
       <c r="B122" s="2"/>
@@ -2688,620 +2609,620 @@
     <row r="123" spans="1:46">
       <c r="A123" s="4"/>
       <c r="B123" s="2"/>
-      <c r="C123" s="11"/>
-      <c r="AB123" s="12"/>
-      <c r="AC123" s="12"/>
-      <c r="AR123" s="17"/>
-      <c r="AS123" s="12"/>
-      <c r="AT123" s="12"/>
+      <c r="C123" s="10"/>
+      <c r="AB123" s="11"/>
+      <c r="AC123" s="11"/>
+      <c r="AR123" s="16"/>
+      <c r="AS123" s="11"/>
+      <c r="AT123" s="11"/>
     </row>
     <row r="124" spans="1:46">
       <c r="A124" s="4"/>
       <c r="B124" s="2"/>
-      <c r="C124" s="11"/>
-      <c r="AB124" s="12"/>
-      <c r="AC124" s="12"/>
-      <c r="AR124" s="17"/>
-      <c r="AS124" s="12"/>
-      <c r="AT124" s="12"/>
+      <c r="C124" s="10"/>
+      <c r="AB124" s="11"/>
+      <c r="AC124" s="11"/>
+      <c r="AR124" s="16"/>
+      <c r="AS124" s="11"/>
+      <c r="AT124" s="11"/>
     </row>
     <row r="125" spans="1:46">
       <c r="A125" s="4"/>
       <c r="B125" s="2"/>
-      <c r="C125" s="11"/>
-      <c r="AB125" s="12"/>
-      <c r="AC125" s="12"/>
-      <c r="AR125" s="17"/>
-      <c r="AS125" s="12"/>
-      <c r="AT125" s="12"/>
+      <c r="C125" s="10"/>
+      <c r="AB125" s="11"/>
+      <c r="AC125" s="11"/>
+      <c r="AR125" s="16"/>
+      <c r="AS125" s="11"/>
+      <c r="AT125" s="11"/>
     </row>
     <row r="126" spans="1:46">
       <c r="A126" s="4"/>
       <c r="B126" s="2"/>
-      <c r="C126" s="11"/>
-      <c r="Z126" s="12"/>
-      <c r="AA126" s="12"/>
-      <c r="AB126" s="12"/>
-      <c r="AC126" s="12"/>
-      <c r="AR126" s="17"/>
-      <c r="AS126" s="12"/>
-      <c r="AT126" s="12"/>
+      <c r="C126" s="10"/>
+      <c r="Z126" s="11"/>
+      <c r="AA126" s="11"/>
+      <c r="AB126" s="11"/>
+      <c r="AC126" s="11"/>
+      <c r="AR126" s="16"/>
+      <c r="AS126" s="11"/>
+      <c r="AT126" s="11"/>
     </row>
     <row r="127" spans="1:46">
       <c r="A127" s="4"/>
       <c r="B127" s="2"/>
-      <c r="C127" s="11"/>
-      <c r="Z127" s="12"/>
-      <c r="AA127" s="12"/>
-      <c r="AB127" s="12"/>
-      <c r="AC127" s="12"/>
-      <c r="AR127" s="17"/>
-      <c r="AS127" s="12"/>
-      <c r="AT127" s="12"/>
+      <c r="C127" s="10"/>
+      <c r="Z127" s="11"/>
+      <c r="AA127" s="11"/>
+      <c r="AB127" s="11"/>
+      <c r="AC127" s="11"/>
+      <c r="AR127" s="16"/>
+      <c r="AS127" s="11"/>
+      <c r="AT127" s="11"/>
     </row>
     <row r="128" spans="1:46">
       <c r="A128" s="4"/>
       <c r="B128" s="2"/>
-      <c r="C128" s="11"/>
-      <c r="Z128" s="12"/>
-      <c r="AA128" s="12"/>
-      <c r="AB128" s="12"/>
-      <c r="AC128" s="12"/>
-      <c r="AR128" s="17"/>
-      <c r="AS128" s="12"/>
-      <c r="AT128" s="12"/>
+      <c r="C128" s="10"/>
+      <c r="Z128" s="11"/>
+      <c r="AA128" s="11"/>
+      <c r="AB128" s="11"/>
+      <c r="AC128" s="11"/>
+      <c r="AR128" s="16"/>
+      <c r="AS128" s="11"/>
+      <c r="AT128" s="11"/>
     </row>
     <row r="129" spans="1:46">
       <c r="A129" s="4"/>
       <c r="B129" s="2"/>
-      <c r="C129" s="11"/>
+      <c r="C129" s="10"/>
       <c r="D129" s="2"/>
-      <c r="Z129" s="12"/>
-      <c r="AA129" s="12"/>
-      <c r="AB129" s="12"/>
+      <c r="Z129" s="11"/>
+      <c r="AA129" s="11"/>
+      <c r="AB129" s="11"/>
     </row>
     <row r="130" spans="1:46">
       <c r="A130" s="4"/>
       <c r="B130" s="2"/>
-      <c r="C130" s="11"/>
-      <c r="Z130" s="11"/>
-      <c r="AA130" s="11"/>
-      <c r="AB130" s="12"/>
-      <c r="AC130" s="12"/>
-      <c r="AR130" s="17"/>
-      <c r="AS130" s="12"/>
-      <c r="AT130" s="12"/>
+      <c r="C130" s="10"/>
+      <c r="Z130" s="10"/>
+      <c r="AA130" s="10"/>
+      <c r="AB130" s="11"/>
+      <c r="AC130" s="11"/>
+      <c r="AR130" s="16"/>
+      <c r="AS130" s="11"/>
+      <c r="AT130" s="11"/>
     </row>
     <row r="131" spans="1:46">
       <c r="A131" s="4"/>
       <c r="B131" s="2"/>
-      <c r="C131" s="11"/>
-      <c r="Z131" s="11"/>
-      <c r="AA131" s="11"/>
-      <c r="AB131" s="12"/>
-      <c r="AC131" s="12"/>
-      <c r="AR131" s="17"/>
-      <c r="AS131" s="12"/>
-      <c r="AT131" s="12"/>
+      <c r="C131" s="10"/>
+      <c r="Z131" s="10"/>
+      <c r="AA131" s="10"/>
+      <c r="AB131" s="11"/>
+      <c r="AC131" s="11"/>
+      <c r="AR131" s="16"/>
+      <c r="AS131" s="11"/>
+      <c r="AT131" s="11"/>
     </row>
     <row r="132" spans="1:46">
       <c r="A132" s="4"/>
       <c r="B132" s="2"/>
-      <c r="C132" s="11"/>
-      <c r="Z132" s="11"/>
-      <c r="AA132" s="11"/>
-      <c r="AB132" s="12"/>
-      <c r="AC132" s="12"/>
+      <c r="C132" s="10"/>
+      <c r="Z132" s="10"/>
+      <c r="AA132" s="10"/>
+      <c r="AB132" s="11"/>
+      <c r="AC132" s="11"/>
     </row>
     <row r="133" spans="1:46">
       <c r="A133" s="4"/>
       <c r="B133" s="2"/>
-      <c r="C133" s="11"/>
-      <c r="T133" s="12"/>
-      <c r="U133" s="12"/>
-      <c r="Z133" s="12"/>
-      <c r="AA133" s="12"/>
-      <c r="AB133" s="12"/>
-      <c r="AC133" s="12"/>
+      <c r="C133" s="10"/>
+      <c r="T133" s="11"/>
+      <c r="U133" s="11"/>
+      <c r="Z133" s="11"/>
+      <c r="AA133" s="11"/>
+      <c r="AB133" s="11"/>
+      <c r="AC133" s="11"/>
     </row>
     <row r="134" spans="1:46">
       <c r="A134" s="4"/>
       <c r="B134" s="2"/>
-      <c r="C134" s="11"/>
-      <c r="T134" s="12"/>
-      <c r="U134" s="12"/>
-      <c r="Z134" s="12"/>
-      <c r="AA134" s="12"/>
-      <c r="AB134" s="12"/>
-      <c r="AC134" s="12"/>
+      <c r="C134" s="10"/>
+      <c r="T134" s="11"/>
+      <c r="U134" s="11"/>
+      <c r="Z134" s="11"/>
+      <c r="AA134" s="11"/>
+      <c r="AB134" s="11"/>
+      <c r="AC134" s="11"/>
     </row>
     <row r="135" spans="1:46">
       <c r="A135" s="4"/>
       <c r="B135" s="2"/>
-      <c r="C135" s="11"/>
-      <c r="T135" s="12"/>
-      <c r="U135" s="12"/>
-      <c r="Z135" s="12"/>
-      <c r="AA135" s="12"/>
-      <c r="AB135" s="12"/>
-      <c r="AC135" s="12"/>
-      <c r="AR135" s="17"/>
-      <c r="AS135" s="12"/>
-      <c r="AT135" s="12"/>
+      <c r="C135" s="10"/>
+      <c r="T135" s="11"/>
+      <c r="U135" s="11"/>
+      <c r="Z135" s="11"/>
+      <c r="AA135" s="11"/>
+      <c r="AB135" s="11"/>
+      <c r="AC135" s="11"/>
+      <c r="AR135" s="16"/>
+      <c r="AS135" s="11"/>
+      <c r="AT135" s="11"/>
     </row>
     <row r="136" spans="1:46">
       <c r="A136" s="4"/>
       <c r="B136" s="2"/>
-      <c r="C136" s="11"/>
+      <c r="C136" s="10"/>
       <c r="D136" s="2"/>
-      <c r="T136" s="12"/>
-      <c r="U136" s="12"/>
-      <c r="Z136" s="12"/>
-      <c r="AA136" s="12"/>
-      <c r="AB136" s="12"/>
+      <c r="T136" s="11"/>
+      <c r="U136" s="11"/>
+      <c r="Z136" s="11"/>
+      <c r="AA136" s="11"/>
+      <c r="AB136" s="11"/>
     </row>
     <row r="137" spans="1:46">
       <c r="A137" s="4"/>
       <c r="B137" s="2"/>
-      <c r="C137" s="11"/>
+      <c r="C137" s="10"/>
       <c r="D137" s="2"/>
-      <c r="T137" s="12"/>
-      <c r="U137" s="12"/>
-      <c r="Z137" s="13"/>
-      <c r="AA137" s="13"/>
-      <c r="AB137" s="13"/>
-      <c r="AC137" s="13"/>
+      <c r="T137" s="11"/>
+      <c r="U137" s="11"/>
+      <c r="Z137" s="12"/>
+      <c r="AA137" s="12"/>
+      <c r="AB137" s="12"/>
+      <c r="AC137" s="12"/>
     </row>
     <row r="138" spans="1:46">
       <c r="A138" s="4"/>
       <c r="B138" s="2"/>
-      <c r="C138" s="11"/>
+      <c r="C138" s="10"/>
       <c r="D138" s="2"/>
-      <c r="T138" s="12"/>
-      <c r="U138" s="12"/>
-      <c r="Z138" s="13"/>
-      <c r="AA138" s="13"/>
-      <c r="AB138" s="13"/>
-      <c r="AC138" s="13"/>
+      <c r="T138" s="11"/>
+      <c r="U138" s="11"/>
+      <c r="Z138" s="12"/>
+      <c r="AA138" s="12"/>
+      <c r="AB138" s="12"/>
+      <c r="AC138" s="12"/>
     </row>
     <row r="139" spans="1:46" s="5" customFormat="1">
-      <c r="A139" s="9"/>
+      <c r="A139" s="8"/>
       <c r="B139" s="6"/>
-      <c r="C139" s="16"/>
-      <c r="G139" s="17"/>
-      <c r="H139" s="16"/>
+      <c r="C139" s="15"/>
+      <c r="G139" s="16"/>
+      <c r="H139" s="15"/>
       <c r="T139"/>
       <c r="U139"/>
-      <c r="Z139" s="17"/>
-      <c r="AA139" s="17"/>
+      <c r="Z139" s="16"/>
+      <c r="AA139" s="16"/>
     </row>
     <row r="140" spans="1:46" s="5" customFormat="1">
-      <c r="A140" s="9"/>
+      <c r="A140" s="8"/>
       <c r="B140" s="6"/>
-      <c r="C140" s="16"/>
-      <c r="G140" s="17"/>
-      <c r="H140" s="16"/>
+      <c r="C140" s="15"/>
+      <c r="G140" s="16"/>
+      <c r="H140" s="15"/>
       <c r="T140"/>
       <c r="U140"/>
-      <c r="Z140" s="17"/>
-      <c r="AA140" s="17"/>
+      <c r="Z140" s="16"/>
+      <c r="AA140" s="16"/>
     </row>
     <row r="141" spans="1:46" s="5" customFormat="1">
-      <c r="A141" s="9"/>
+      <c r="A141" s="8"/>
       <c r="B141" s="6"/>
-      <c r="C141" s="16"/>
-      <c r="G141" s="17"/>
-      <c r="H141" s="16"/>
+      <c r="C141" s="15"/>
+      <c r="G141" s="16"/>
+      <c r="H141" s="15"/>
       <c r="T141"/>
       <c r="U141"/>
-      <c r="Z141" s="17"/>
-      <c r="AA141" s="17"/>
+      <c r="Z141" s="16"/>
+      <c r="AA141" s="16"/>
     </row>
     <row r="142" spans="1:46" s="5" customFormat="1">
-      <c r="A142" s="9"/>
+      <c r="A142" s="8"/>
       <c r="B142" s="6"/>
-      <c r="C142" s="16"/>
+      <c r="C142" s="15"/>
       <c r="D142" s="6"/>
-      <c r="G142" s="17"/>
-      <c r="H142" s="16"/>
-      <c r="T142" s="16"/>
+      <c r="G142" s="16"/>
+      <c r="H142" s="15"/>
+      <c r="T142" s="15"/>
       <c r="U142"/>
-      <c r="Z142" s="17"/>
-      <c r="AA142" s="17"/>
+      <c r="Z142" s="16"/>
+      <c r="AA142" s="16"/>
       <c r="AC142"/>
     </row>
     <row r="143" spans="1:46">
       <c r="A143" s="4"/>
       <c r="B143" s="2"/>
-      <c r="C143" s="11"/>
+      <c r="C143" s="10"/>
       <c r="D143" s="2"/>
-      <c r="G143" s="12"/>
-      <c r="H143" s="11"/>
-      <c r="Z143" s="13"/>
-      <c r="AA143" s="13"/>
-      <c r="AB143" s="14"/>
+      <c r="G143" s="11"/>
+      <c r="H143" s="10"/>
+      <c r="Z143" s="12"/>
+      <c r="AA143" s="12"/>
+      <c r="AB143" s="13"/>
     </row>
     <row r="144" spans="1:46">
       <c r="A144" s="4"/>
       <c r="B144" s="2"/>
-      <c r="C144" s="11"/>
+      <c r="C144" s="10"/>
       <c r="D144" s="2"/>
-      <c r="G144" s="12"/>
-      <c r="H144" s="11"/>
-      <c r="Z144" s="13"/>
-      <c r="AA144" s="13"/>
-      <c r="AB144" s="13"/>
+      <c r="G144" s="11"/>
+      <c r="H144" s="10"/>
+      <c r="Z144" s="12"/>
+      <c r="AA144" s="12"/>
+      <c r="AB144" s="12"/>
     </row>
     <row r="145" spans="1:30">
       <c r="A145" s="4"/>
       <c r="B145" s="2"/>
-      <c r="C145" s="11"/>
+      <c r="C145" s="10"/>
       <c r="D145" s="2"/>
-      <c r="G145" s="12"/>
-      <c r="H145" s="11"/>
-      <c r="Z145" s="13"/>
-      <c r="AA145" s="13"/>
-      <c r="AB145" s="14"/>
+      <c r="G145" s="11"/>
+      <c r="H145" s="10"/>
+      <c r="Z145" s="12"/>
+      <c r="AA145" s="12"/>
+      <c r="AB145" s="13"/>
     </row>
     <row r="146" spans="1:30">
       <c r="A146" s="4"/>
       <c r="B146" s="2"/>
-      <c r="C146" s="11"/>
+      <c r="C146" s="10"/>
       <c r="D146" s="2"/>
-      <c r="H146" s="11"/>
-      <c r="Z146" s="13"/>
-      <c r="AA146" s="13"/>
-      <c r="AB146" s="13"/>
+      <c r="H146" s="10"/>
+      <c r="Z146" s="12"/>
+      <c r="AA146" s="12"/>
+      <c r="AB146" s="12"/>
     </row>
     <row r="147" spans="1:30">
       <c r="A147" s="4"/>
       <c r="B147" s="2"/>
-      <c r="C147" s="11"/>
+      <c r="C147" s="10"/>
       <c r="D147" s="2"/>
-      <c r="Z147" s="13"/>
-      <c r="AA147" s="13"/>
-      <c r="AB147" s="13"/>
-      <c r="AD147" s="15"/>
+      <c r="Z147" s="12"/>
+      <c r="AA147" s="12"/>
+      <c r="AB147" s="12"/>
+      <c r="AD147" s="14"/>
     </row>
     <row r="148" spans="1:30">
       <c r="A148" s="4"/>
       <c r="B148" s="2"/>
-      <c r="C148" s="11"/>
+      <c r="C148" s="10"/>
       <c r="D148" s="2"/>
-      <c r="Z148" s="13"/>
-      <c r="AA148" s="13"/>
-      <c r="AB148" s="13"/>
+      <c r="Z148" s="12"/>
+      <c r="AA148" s="12"/>
+      <c r="AB148" s="12"/>
     </row>
     <row r="149" spans="1:30">
-      <c r="B149" s="18"/>
+      <c r="B149" s="17"/>
     </row>
     <row r="150" spans="1:30">
-      <c r="B150" s="18"/>
+      <c r="B150" s="17"/>
     </row>
     <row r="151" spans="1:30">
-      <c r="B151" s="18"/>
+      <c r="B151" s="17"/>
     </row>
     <row r="152" spans="1:30">
-      <c r="B152" s="18"/>
+      <c r="B152" s="17"/>
     </row>
     <row r="153" spans="1:30">
-      <c r="B153" s="18"/>
+      <c r="B153" s="17"/>
     </row>
     <row r="154" spans="1:30">
-      <c r="B154" s="18"/>
+      <c r="B154" s="17"/>
     </row>
     <row r="155" spans="1:30">
-      <c r="B155" s="18"/>
+      <c r="B155" s="17"/>
       <c r="D155" s="2"/>
     </row>
     <row r="156" spans="1:30">
-      <c r="B156" s="18"/>
+      <c r="B156" s="17"/>
     </row>
     <row r="157" spans="1:30">
-      <c r="B157" s="18"/>
+      <c r="B157" s="17"/>
     </row>
     <row r="158" spans="1:30">
-      <c r="B158" s="18"/>
+      <c r="B158" s="17"/>
     </row>
     <row r="159" spans="1:30">
-      <c r="B159" s="18"/>
+      <c r="B159" s="17"/>
     </row>
     <row r="160" spans="1:30">
-      <c r="B160" s="18"/>
+      <c r="B160" s="17"/>
     </row>
     <row r="161" spans="2:4">
-      <c r="B161" s="18"/>
+      <c r="B161" s="17"/>
     </row>
     <row r="162" spans="2:4">
-      <c r="B162" s="18"/>
+      <c r="B162" s="17"/>
       <c r="D162" s="2"/>
     </row>
     <row r="163" spans="2:4">
-      <c r="B163" s="18"/>
+      <c r="B163" s="17"/>
     </row>
     <row r="164" spans="2:4">
-      <c r="B164" s="18"/>
+      <c r="B164" s="17"/>
     </row>
     <row r="165" spans="2:4">
-      <c r="B165" s="18"/>
+      <c r="B165" s="17"/>
     </row>
     <row r="166" spans="2:4">
-      <c r="B166" s="18"/>
+      <c r="B166" s="17"/>
     </row>
     <row r="167" spans="2:4">
-      <c r="B167" s="18"/>
+      <c r="B167" s="17"/>
     </row>
     <row r="168" spans="2:4">
-      <c r="B168" s="18"/>
+      <c r="B168" s="17"/>
     </row>
     <row r="169" spans="2:4">
-      <c r="B169" s="18"/>
+      <c r="B169" s="17"/>
       <c r="D169" s="2"/>
     </row>
     <row r="170" spans="2:4">
-      <c r="B170" s="18"/>
+      <c r="B170" s="17"/>
     </row>
     <row r="171" spans="2:4">
-      <c r="B171" s="18"/>
+      <c r="B171" s="17"/>
     </row>
     <row r="172" spans="2:4">
-      <c r="B172" s="18"/>
+      <c r="B172" s="17"/>
     </row>
     <row r="173" spans="2:4">
-      <c r="B173" s="18"/>
+      <c r="B173" s="17"/>
     </row>
     <row r="174" spans="2:4">
-      <c r="B174" s="18"/>
+      <c r="B174" s="17"/>
     </row>
     <row r="175" spans="2:4">
-      <c r="B175" s="18"/>
+      <c r="B175" s="17"/>
     </row>
     <row r="176" spans="2:4">
-      <c r="B176" s="18"/>
+      <c r="B176" s="17"/>
       <c r="D176" s="2"/>
     </row>
     <row r="177" spans="2:4">
-      <c r="B177" s="18"/>
+      <c r="B177" s="17"/>
     </row>
     <row r="178" spans="2:4">
-      <c r="B178" s="18"/>
+      <c r="B178" s="17"/>
     </row>
     <row r="179" spans="2:4">
-      <c r="B179" s="18"/>
+      <c r="B179" s="17"/>
     </row>
     <row r="180" spans="2:4">
-      <c r="B180" s="18"/>
+      <c r="B180" s="17"/>
     </row>
     <row r="181" spans="2:4">
-      <c r="B181" s="18"/>
+      <c r="B181" s="17"/>
     </row>
     <row r="182" spans="2:4">
-      <c r="B182" s="18"/>
+      <c r="B182" s="17"/>
     </row>
     <row r="183" spans="2:4">
-      <c r="B183" s="18"/>
+      <c r="B183" s="17"/>
       <c r="D183" s="2"/>
     </row>
     <row r="184" spans="2:4">
-      <c r="B184" s="18"/>
+      <c r="B184" s="17"/>
     </row>
     <row r="185" spans="2:4">
-      <c r="B185" s="18"/>
+      <c r="B185" s="17"/>
     </row>
     <row r="186" spans="2:4">
-      <c r="B186" s="18"/>
+      <c r="B186" s="17"/>
     </row>
     <row r="187" spans="2:4">
-      <c r="B187" s="18"/>
+      <c r="B187" s="17"/>
     </row>
     <row r="188" spans="2:4">
-      <c r="B188" s="18"/>
+      <c r="B188" s="17"/>
     </row>
     <row r="189" spans="2:4">
-      <c r="B189" s="18"/>
+      <c r="B189" s="17"/>
     </row>
     <row r="190" spans="2:4">
-      <c r="B190" s="18"/>
+      <c r="B190" s="17"/>
       <c r="D190" s="2"/>
     </row>
     <row r="191" spans="2:4">
-      <c r="B191" s="18"/>
+      <c r="B191" s="17"/>
     </row>
     <row r="192" spans="2:4">
-      <c r="B192" s="18"/>
+      <c r="B192" s="17"/>
     </row>
     <row r="193" spans="2:94">
-      <c r="B193" s="18"/>
+      <c r="B193" s="17"/>
     </row>
     <row r="194" spans="2:94">
-      <c r="B194" s="18"/>
+      <c r="B194" s="17"/>
     </row>
     <row r="195" spans="2:94">
-      <c r="B195" s="18"/>
+      <c r="B195" s="17"/>
     </row>
     <row r="196" spans="2:94">
-      <c r="B196" s="18"/>
+      <c r="B196" s="17"/>
     </row>
     <row r="197" spans="2:94">
-      <c r="B197" s="18"/>
+      <c r="B197" s="17"/>
       <c r="D197" s="2"/>
     </row>
     <row r="198" spans="2:94">
-      <c r="B198" s="18"/>
+      <c r="B198" s="17"/>
     </row>
     <row r="199" spans="2:94">
-      <c r="B199" s="18"/>
+      <c r="B199" s="17"/>
     </row>
     <row r="200" spans="2:94">
-      <c r="B200" s="18"/>
+      <c r="B200" s="17"/>
     </row>
     <row r="201" spans="2:94">
-      <c r="B201" s="18"/>
+      <c r="B201" s="17"/>
     </row>
     <row r="202" spans="2:94">
-      <c r="B202" s="18"/>
+      <c r="B202" s="17"/>
     </row>
     <row r="203" spans="2:94">
-      <c r="B203" s="18"/>
+      <c r="B203" s="17"/>
     </row>
     <row r="204" spans="2:94">
-      <c r="B204" s="18"/>
+      <c r="B204" s="17"/>
       <c r="D204" s="2"/>
     </row>
     <row r="205" spans="2:94">
       <c r="B205" s="2"/>
-      <c r="AS205" s="8"/>
-      <c r="CP205" s="8"/>
+      <c r="AS205" s="7"/>
+      <c r="CP205" s="7"/>
     </row>
     <row r="206" spans="2:94">
       <c r="B206" s="2"/>
-      <c r="AS206" s="8"/>
-      <c r="CP206" s="8"/>
+      <c r="AS206" s="7"/>
+      <c r="CP206" s="7"/>
     </row>
     <row r="207" spans="2:94">
       <c r="B207" s="2"/>
-      <c r="AS207" s="8"/>
-      <c r="CP207" s="8"/>
+      <c r="AS207" s="7"/>
+      <c r="CP207" s="7"/>
     </row>
     <row r="208" spans="2:94">
       <c r="B208" s="2"/>
-      <c r="AS208" s="8"/>
-      <c r="CP208" s="8"/>
+      <c r="AS208" s="7"/>
+      <c r="CP208" s="7"/>
     </row>
     <row r="209" spans="2:94">
       <c r="B209" s="2"/>
-      <c r="AS209" s="8"/>
-      <c r="CP209" s="8"/>
+      <c r="AS209" s="7"/>
+      <c r="CP209" s="7"/>
     </row>
     <row r="210" spans="2:94">
       <c r="B210" s="2"/>
-      <c r="AS210" s="8"/>
-      <c r="CP210" s="8"/>
+      <c r="AS210" s="7"/>
+      <c r="CP210" s="7"/>
     </row>
     <row r="211" spans="2:94">
       <c r="B211" s="2"/>
-      <c r="AS211" s="8"/>
-      <c r="CP211" s="8"/>
+      <c r="AS211" s="7"/>
+      <c r="CP211" s="7"/>
     </row>
     <row r="212" spans="2:94">
       <c r="B212" s="2"/>
-      <c r="AS212" s="8"/>
-      <c r="CP212" s="8"/>
+      <c r="AS212" s="7"/>
+      <c r="CP212" s="7"/>
     </row>
     <row r="213" spans="2:94">
       <c r="B213" s="2"/>
-      <c r="AS213" s="8"/>
-      <c r="CP213" s="8"/>
+      <c r="AS213" s="7"/>
+      <c r="CP213" s="7"/>
     </row>
     <row r="214" spans="2:94">
       <c r="B214" s="2"/>
-      <c r="AS214" s="8"/>
-      <c r="CP214" s="8"/>
+      <c r="AS214" s="7"/>
+      <c r="CP214" s="7"/>
     </row>
     <row r="215" spans="2:94">
       <c r="B215" s="2"/>
-      <c r="AS215" s="8"/>
-      <c r="CP215" s="8"/>
+      <c r="AS215" s="7"/>
+      <c r="CP215" s="7"/>
     </row>
     <row r="216" spans="2:94">
       <c r="B216" s="2"/>
-      <c r="AS216" s="8"/>
-      <c r="CP216" s="8"/>
+      <c r="AS216" s="7"/>
+      <c r="CP216" s="7"/>
     </row>
     <row r="217" spans="2:94">
       <c r="B217" s="2"/>
-      <c r="AS217" s="8"/>
-      <c r="CP217" s="8"/>
+      <c r="AS217" s="7"/>
+      <c r="CP217" s="7"/>
     </row>
     <row r="218" spans="2:94">
       <c r="B218" s="2"/>
-      <c r="AS218" s="8"/>
-      <c r="CP218" s="8"/>
+      <c r="AS218" s="7"/>
+      <c r="CP218" s="7"/>
     </row>
     <row r="219" spans="2:94">
       <c r="B219" s="2"/>
-      <c r="AS219" s="8"/>
-      <c r="CP219" s="8"/>
+      <c r="AS219" s="7"/>
+      <c r="CP219" s="7"/>
     </row>
     <row r="220" spans="2:94">
       <c r="B220" s="2"/>
-      <c r="AS220" s="8"/>
-      <c r="CP220" s="8"/>
+      <c r="AS220" s="7"/>
+      <c r="CP220" s="7"/>
     </row>
     <row r="221" spans="2:94">
       <c r="B221" s="2"/>
-      <c r="AS221" s="8"/>
-      <c r="CP221" s="8"/>
+      <c r="AS221" s="7"/>
+      <c r="CP221" s="7"/>
     </row>
     <row r="222" spans="2:94">
       <c r="B222" s="2"/>
-      <c r="AS222" s="8"/>
-      <c r="CP222" s="8"/>
+      <c r="AS222" s="7"/>
+      <c r="CP222" s="7"/>
     </row>
     <row r="223" spans="2:94">
       <c r="B223" s="2"/>
-      <c r="AS223" s="8"/>
-      <c r="CP223" s="8"/>
+      <c r="AS223" s="7"/>
+      <c r="CP223" s="7"/>
     </row>
     <row r="224" spans="2:94">
       <c r="B224" s="2"/>
-      <c r="AS224" s="8"/>
-      <c r="CP224" s="8"/>
+      <c r="AS224" s="7"/>
+      <c r="CP224" s="7"/>
     </row>
     <row r="225" spans="1:94">
       <c r="B225" s="2"/>
-      <c r="AS225" s="8"/>
-      <c r="CP225" s="8"/>
+      <c r="AS225" s="7"/>
+      <c r="CP225" s="7"/>
     </row>
     <row r="226" spans="1:94">
       <c r="B226" s="2"/>
-      <c r="AS226" s="8"/>
-      <c r="CP226" s="8"/>
+      <c r="AS226" s="7"/>
+      <c r="CP226" s="7"/>
     </row>
     <row r="227" spans="1:94">
       <c r="B227" s="2"/>
-      <c r="AS227" s="8"/>
-      <c r="CP227" s="8"/>
+      <c r="AS227" s="7"/>
+      <c r="CP227" s="7"/>
     </row>
     <row r="228" spans="1:94">
       <c r="B228" s="2"/>
-      <c r="AS228" s="8"/>
-      <c r="CP228" s="8"/>
+      <c r="AS228" s="7"/>
+      <c r="CP228" s="7"/>
     </row>
     <row r="229" spans="1:94">
       <c r="B229" s="2"/>
-      <c r="AS229" s="8"/>
-      <c r="CP229" s="8"/>
+      <c r="AS229" s="7"/>
+      <c r="CP229" s="7"/>
     </row>
     <row r="230" spans="1:94">
       <c r="B230" s="2"/>
-      <c r="AS230" s="8"/>
-      <c r="CP230" s="8"/>
+      <c r="AS230" s="7"/>
+      <c r="CP230" s="7"/>
     </row>
     <row r="231" spans="1:94">
       <c r="B231" s="2"/>
-      <c r="AS231" s="8"/>
-      <c r="CP231" s="8"/>
+      <c r="AS231" s="7"/>
+      <c r="CP231" s="7"/>
     </row>
     <row r="232" spans="1:94">
       <c r="B232" s="2"/>
-      <c r="AS232" s="8"/>
-      <c r="CP232" s="8"/>
+      <c r="AS232" s="7"/>
+      <c r="CP232" s="7"/>
     </row>
     <row r="233" spans="1:94">
       <c r="B233" s="2"/>
-      <c r="AS233" s="8"/>
-      <c r="CP233" s="8"/>
+      <c r="AS233" s="7"/>
+      <c r="CP233" s="7"/>
     </row>
     <row r="234" spans="1:94">
       <c r="B234" s="2"/>
-      <c r="AS234" s="8"/>
-      <c r="CP234" s="8"/>
+      <c r="AS234" s="7"/>
+      <c r="CP234" s="7"/>
     </row>
     <row r="235" spans="1:94">
       <c r="B235" s="2"/>
-      <c r="AS235" s="8"/>
-      <c r="CP235" s="8"/>
+      <c r="AS235" s="7"/>
+      <c r="CP235" s="7"/>
     </row>
     <row r="236" spans="1:94">
       <c r="A236" s="4"/>
@@ -3605,214 +3526,214 @@
       <c r="D335" s="2"/>
     </row>
     <row r="336" spans="1:96">
-      <c r="A336" s="22"/>
-      <c r="B336" s="19"/>
-      <c r="CQ336" s="20"/>
-      <c r="CR336" s="20"/>
+      <c r="A336" s="21"/>
+      <c r="B336" s="18"/>
+      <c r="CQ336" s="19"/>
+      <c r="CR336" s="19"/>
     </row>
     <row r="337" spans="1:96">
-      <c r="A337" s="22"/>
-      <c r="B337" s="19"/>
-      <c r="CQ337" s="20"/>
-      <c r="CR337" s="20"/>
+      <c r="A337" s="21"/>
+      <c r="B337" s="18"/>
+      <c r="CQ337" s="19"/>
+      <c r="CR337" s="19"/>
     </row>
     <row r="338" spans="1:96">
-      <c r="A338" s="22"/>
-      <c r="B338" s="19"/>
-      <c r="CQ338" s="20"/>
-      <c r="CR338" s="20"/>
+      <c r="A338" s="21"/>
+      <c r="B338" s="18"/>
+      <c r="CQ338" s="19"/>
+      <c r="CR338" s="19"/>
     </row>
     <row r="339" spans="1:96">
-      <c r="A339" s="22"/>
-      <c r="B339" s="19"/>
-      <c r="CQ339" s="20"/>
-      <c r="CR339" s="20"/>
+      <c r="A339" s="21"/>
+      <c r="B339" s="18"/>
+      <c r="CQ339" s="19"/>
+      <c r="CR339" s="19"/>
     </row>
     <row r="340" spans="1:96">
-      <c r="A340" s="22"/>
-      <c r="B340" s="19"/>
-      <c r="CQ340" s="20"/>
-      <c r="CR340" s="20"/>
+      <c r="A340" s="21"/>
+      <c r="B340" s="18"/>
+      <c r="CQ340" s="19"/>
+      <c r="CR340" s="19"/>
     </row>
     <row r="341" spans="1:96">
-      <c r="A341" s="22"/>
-      <c r="B341" s="19"/>
-      <c r="CQ341" s="20"/>
-      <c r="CR341" s="20"/>
+      <c r="A341" s="21"/>
+      <c r="B341" s="18"/>
+      <c r="CQ341" s="19"/>
+      <c r="CR341" s="19"/>
     </row>
     <row r="342" spans="1:96">
-      <c r="A342" s="22"/>
-      <c r="B342" s="19"/>
-      <c r="CQ342" s="20"/>
-      <c r="CR342" s="20"/>
+      <c r="A342" s="21"/>
+      <c r="B342" s="18"/>
+      <c r="CQ342" s="19"/>
+      <c r="CR342" s="19"/>
     </row>
     <row r="343" spans="1:96">
-      <c r="A343" s="22"/>
-      <c r="B343" s="19"/>
-      <c r="CQ343" s="20"/>
-      <c r="CR343" s="20"/>
+      <c r="A343" s="21"/>
+      <c r="B343" s="18"/>
+      <c r="CQ343" s="19"/>
+      <c r="CR343" s="19"/>
     </row>
     <row r="344" spans="1:96">
-      <c r="A344" s="22"/>
-      <c r="B344" s="19"/>
-      <c r="CQ344" s="20"/>
-      <c r="CR344" s="20"/>
+      <c r="A344" s="21"/>
+      <c r="B344" s="18"/>
+      <c r="CQ344" s="19"/>
+      <c r="CR344" s="19"/>
     </row>
     <row r="345" spans="1:96">
-      <c r="A345" s="22"/>
-      <c r="B345" s="19"/>
-      <c r="CQ345" s="20"/>
-      <c r="CR345" s="20"/>
+      <c r="A345" s="21"/>
+      <c r="B345" s="18"/>
+      <c r="CQ345" s="19"/>
+      <c r="CR345" s="19"/>
     </row>
     <row r="346" spans="1:96">
-      <c r="A346" s="22"/>
-      <c r="B346" s="19"/>
-      <c r="CQ346" s="20"/>
-      <c r="CR346" s="20"/>
+      <c r="A346" s="21"/>
+      <c r="B346" s="18"/>
+      <c r="CQ346" s="19"/>
+      <c r="CR346" s="19"/>
     </row>
     <row r="347" spans="1:96">
-      <c r="A347" s="22"/>
-      <c r="B347" s="19"/>
-      <c r="CQ347" s="20"/>
-      <c r="CR347" s="20"/>
+      <c r="A347" s="21"/>
+      <c r="B347" s="18"/>
+      <c r="CQ347" s="19"/>
+      <c r="CR347" s="19"/>
     </row>
     <row r="348" spans="1:96">
-      <c r="A348" s="22"/>
-      <c r="B348" s="19"/>
-      <c r="CQ348" s="20"/>
-      <c r="CR348" s="20"/>
+      <c r="A348" s="21"/>
+      <c r="B348" s="18"/>
+      <c r="CQ348" s="19"/>
+      <c r="CR348" s="19"/>
     </row>
     <row r="349" spans="1:96">
-      <c r="A349" s="22"/>
-      <c r="B349" s="19"/>
-      <c r="CQ349" s="20"/>
-      <c r="CR349" s="20"/>
+      <c r="A349" s="21"/>
+      <c r="B349" s="18"/>
+      <c r="CQ349" s="19"/>
+      <c r="CR349" s="19"/>
     </row>
     <row r="350" spans="1:96">
-      <c r="A350" s="22"/>
-      <c r="B350" s="19"/>
-      <c r="CQ350" s="20"/>
-      <c r="CR350" s="20"/>
+      <c r="A350" s="21"/>
+      <c r="B350" s="18"/>
+      <c r="CQ350" s="19"/>
+      <c r="CR350" s="19"/>
     </row>
     <row r="351" spans="1:96">
-      <c r="A351" s="22"/>
-      <c r="B351" s="19"/>
-      <c r="CQ351" s="20"/>
-      <c r="CR351" s="20"/>
+      <c r="A351" s="21"/>
+      <c r="B351" s="18"/>
+      <c r="CQ351" s="19"/>
+      <c r="CR351" s="19"/>
     </row>
     <row r="352" spans="1:96">
-      <c r="A352" s="22"/>
-      <c r="B352" s="19"/>
-      <c r="CQ352" s="20"/>
-      <c r="CR352" s="20"/>
+      <c r="A352" s="21"/>
+      <c r="B352" s="18"/>
+      <c r="CQ352" s="19"/>
+      <c r="CR352" s="19"/>
     </row>
     <row r="353" spans="1:96">
-      <c r="A353" s="22"/>
-      <c r="B353" s="19"/>
-      <c r="CQ353" s="20"/>
-      <c r="CR353" s="20"/>
+      <c r="A353" s="21"/>
+      <c r="B353" s="18"/>
+      <c r="CQ353" s="19"/>
+      <c r="CR353" s="19"/>
     </row>
     <row r="354" spans="1:96">
-      <c r="A354" s="22"/>
-      <c r="B354" s="19"/>
-      <c r="CQ354" s="20"/>
-      <c r="CR354" s="20"/>
+      <c r="A354" s="21"/>
+      <c r="B354" s="18"/>
+      <c r="CQ354" s="19"/>
+      <c r="CR354" s="19"/>
     </row>
     <row r="355" spans="1:96">
-      <c r="A355" s="22"/>
-      <c r="B355" s="19"/>
-      <c r="CQ355" s="20"/>
-      <c r="CR355" s="20"/>
+      <c r="A355" s="21"/>
+      <c r="B355" s="18"/>
+      <c r="CQ355" s="19"/>
+      <c r="CR355" s="19"/>
     </row>
     <row r="356" spans="1:96">
-      <c r="A356" s="22"/>
-      <c r="B356" s="19"/>
-      <c r="CQ356" s="20"/>
-      <c r="CR356" s="20"/>
+      <c r="A356" s="21"/>
+      <c r="B356" s="18"/>
+      <c r="CQ356" s="19"/>
+      <c r="CR356" s="19"/>
     </row>
     <row r="357" spans="1:96">
-      <c r="A357" s="22"/>
-      <c r="B357" s="19"/>
+      <c r="A357" s="21"/>
+      <c r="B357" s="18"/>
     </row>
     <row r="358" spans="1:96">
-      <c r="A358" s="22"/>
-      <c r="B358" s="19"/>
+      <c r="A358" s="21"/>
+      <c r="B358" s="18"/>
     </row>
     <row r="359" spans="1:96">
-      <c r="A359" s="22"/>
-      <c r="B359" s="19"/>
+      <c r="A359" s="21"/>
+      <c r="B359" s="18"/>
     </row>
     <row r="360" spans="1:96">
-      <c r="A360" s="22"/>
-      <c r="B360" s="19"/>
+      <c r="A360" s="21"/>
+      <c r="B360" s="18"/>
     </row>
     <row r="361" spans="1:96">
-      <c r="A361" s="22"/>
-      <c r="B361" s="19"/>
+      <c r="A361" s="21"/>
+      <c r="B361" s="18"/>
     </row>
     <row r="362" spans="1:96">
-      <c r="A362" s="22"/>
-      <c r="B362" s="19"/>
+      <c r="A362" s="21"/>
+      <c r="B362" s="18"/>
     </row>
     <row r="363" spans="1:96">
-      <c r="A363" s="22"/>
-      <c r="B363" s="19"/>
+      <c r="A363" s="21"/>
+      <c r="B363" s="18"/>
     </row>
     <row r="364" spans="1:96">
-      <c r="A364" s="22"/>
-      <c r="B364" s="19"/>
+      <c r="A364" s="21"/>
+      <c r="B364" s="18"/>
     </row>
     <row r="365" spans="1:96">
-      <c r="A365" s="22"/>
-      <c r="B365" s="19"/>
+      <c r="A365" s="21"/>
+      <c r="B365" s="18"/>
     </row>
     <row r="366" spans="1:96">
-      <c r="A366" s="22"/>
-      <c r="B366" s="19"/>
+      <c r="A366" s="21"/>
+      <c r="B366" s="18"/>
     </row>
     <row r="367" spans="1:96">
-      <c r="A367" s="22"/>
-      <c r="B367" s="19"/>
+      <c r="A367" s="21"/>
+      <c r="B367" s="18"/>
     </row>
     <row r="368" spans="1:96">
-      <c r="A368" s="22"/>
-      <c r="B368" s="19"/>
+      <c r="A368" s="21"/>
+      <c r="B368" s="18"/>
     </row>
     <row r="369" spans="1:2">
-      <c r="A369" s="22"/>
-      <c r="B369" s="19"/>
+      <c r="A369" s="21"/>
+      <c r="B369" s="18"/>
     </row>
     <row r="370" spans="1:2">
-      <c r="A370" s="22"/>
-      <c r="B370" s="19"/>
+      <c r="A370" s="21"/>
+      <c r="B370" s="18"/>
     </row>
     <row r="371" spans="1:2">
-      <c r="A371" s="22"/>
-      <c r="B371" s="19"/>
+      <c r="A371" s="21"/>
+      <c r="B371" s="18"/>
     </row>
     <row r="372" spans="1:2">
-      <c r="A372" s="22"/>
-      <c r="B372" s="19"/>
+      <c r="A372" s="21"/>
+      <c r="B372" s="18"/>
     </row>
     <row r="373" spans="1:2">
-      <c r="A373" s="22"/>
-      <c r="B373" s="19"/>
+      <c r="A373" s="21"/>
+      <c r="B373" s="18"/>
     </row>
     <row r="374" spans="1:2">
-      <c r="A374" s="22"/>
-      <c r="B374" s="19"/>
+      <c r="A374" s="21"/>
+      <c r="B374" s="18"/>
     </row>
     <row r="375" spans="1:2">
-      <c r="A375" s="22"/>
-      <c r="B375" s="19"/>
+      <c r="A375" s="21"/>
+      <c r="B375" s="18"/>
     </row>
     <row r="376" spans="1:2">
-      <c r="A376" s="22"/>
-      <c r="B376" s="19"/>
+      <c r="A376" s="21"/>
+      <c r="B376" s="18"/>
     </row>
     <row r="377" spans="1:2">
-      <c r="A377" s="22"/>
-      <c r="B377" s="19"/>
+      <c r="A377" s="21"/>
+      <c r="B377" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>